<commit_message>
Criação do titulo de cada uma das partes do cronograma
Adição dos titulos nas planilhas
</commit_message>
<xml_diff>
--- a/docs/cronograma editavel.xlsx
+++ b/docs/cronograma editavel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b4b0d45743b0940/Faculdade/5 sem/projeto integrador/Easylize-Financas/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\GitHub\Controle-de-Despesas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{8672951D-D7B3-4A6C-997F-A48D944213C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8394FC20-344B-47D9-95DE-F8BA4CB621BD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2448B387-4B76-4786-BE7B-C3A7B7D46A13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{79EF33A3-60E2-4A1D-AA5A-E20F769F513C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{79EF33A3-60E2-4A1D-AA5A-E20F769F513C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>TAREFAS</t>
   </si>
@@ -173,13 +173,19 @@
   </si>
   <si>
     <t>a definir</t>
+  </si>
+  <si>
+    <t>Tarefas da pesquisa</t>
+  </si>
+  <si>
+    <t>Tarefas do software</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +233,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -360,11 +381,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,6 +430,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,7 +461,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,10 +781,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5586467-B6F5-41F0-862B-F00DDC74673E}">
-  <dimension ref="A1:O24"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,115 +799,113 @@
     <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:15" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="23" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="25"/>
-      <c r="N1" s="17" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
+      <c r="N2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="29" t="s">
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="27" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="21" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="N2" s="18" t="s">
+      <c r="L3" s="22"/>
+      <c r="N3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="1" t="s">
+      <c r="O3" s="12"/>
+    </row>
+    <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="N3" s="19" t="s">
+      <c r="L4" s="22"/>
+      <c r="N4" s="19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
@@ -883,13 +920,13 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -901,10 +938,10 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
-        <v>4</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
@@ -919,10 +956,10 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
@@ -937,14 +974,14 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -955,10 +992,10 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
-        <v>7</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -973,15 +1010,15 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
-        <v>8</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -991,15 +1028,15 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1009,15 +1046,15 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
-        <v>10</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1027,16 +1064,16 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1045,10 +1082,10 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1063,17 +1100,17 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -1081,10 +1118,10 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1099,35 +1136,35 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
-        <v>16</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="7"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1135,10 +1172,10 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
-        <v>17</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1146,17 +1183,17 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1165,43 +1202,65 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="9">
+        <v>18</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
     </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K2:L2"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E9CA16-4240-4451-BAA9-90262D6BD0C4}">
-  <dimension ref="A1:O32"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,113 +1273,111 @@
     <col min="15" max="15" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="30" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="N1" s="17" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="N2" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="29" t="s">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="27" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="21" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="N2" s="18" t="s">
+      <c r="L3" s="22"/>
+      <c r="N3" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="1" t="s">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="N3" s="19" t="s">
+      <c r="L4" s="22"/>
+      <c r="N4" s="19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
@@ -1335,10 +1392,10 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
@@ -1353,14 +1410,14 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1371,10 +1428,10 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
-        <v>5</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1389,15 +1446,15 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1407,10 +1464,10 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1425,15 +1482,15 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
-        <v>8</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>36</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="15"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1443,15 +1500,15 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1461,10 +1518,10 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1479,29 +1536,28 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="N14" s="16"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1513,13 +1569,14 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
+      <c r="N15" s="16"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1534,10 +1591,10 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1552,17 +1609,17 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -1570,16 +1627,16 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="7"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1588,10 +1645,10 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1606,10 +1663,10 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1624,41 +1681,43 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="14"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="31"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <v>20</v>
-      </c>
-      <c r="B23" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="14"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="5"/>
@@ -1674,7 +1733,7 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="5"/>
@@ -1690,7 +1749,7 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="5"/>
@@ -1706,7 +1765,7 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="5"/>
@@ -1722,7 +1781,7 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="5"/>
@@ -1738,7 +1797,7 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="5"/>
@@ -1754,7 +1813,7 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="5"/>
@@ -1770,7 +1829,7 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="5"/>
@@ -1786,7 +1845,7 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="5"/>
@@ -1800,17 +1859,35 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>29</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="K2:L2"/>
+  <mergeCells count="9">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C2:L2"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="62" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criado Relatório de Execução de Atividades 2
</commit_message>
<xml_diff>
--- a/docs/cronograma editavel.xlsx
+++ b/docs/cronograma editavel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2448B387-4B76-4786-BE7B-C3A7B7D46A13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5B0042BA-9FDC-4F41-ADD9-1D824788B908}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{79EF33A3-60E2-4A1D-AA5A-E20F769F513C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{79EF33A3-60E2-4A1D-AA5A-E20F769F513C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
@@ -1262,8 +1262,8 @@
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Atualizado Relatorio de execução 3 e cronograma
</commit_message>
<xml_diff>
--- a/docs/cronograma editavel.xlsx
+++ b/docs/cronograma editavel.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\GitHub\Controle-de-Despesas\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NetBeans-12.3\projects\Easylize-Financas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE028F4-9081-4E89-8DD3-5AF5A403D6CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983F1FAE-4BFE-479D-A0CB-90ECF5065867}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{79EF33A3-60E2-4A1D-AA5A-E20F769F513C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{79EF33A3-60E2-4A1D-AA5A-E20F769F513C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
     <sheet name="Projeto" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>TAREFAS</t>
   </si>
@@ -151,15 +151,6 @@
     <t>Design da tela de perfil de usuário</t>
   </si>
   <si>
-    <t>Funções da tela de perfil</t>
-  </si>
-  <si>
-    <t>Design da tela de economias</t>
-  </si>
-  <si>
-    <t>Funções da tela de economias</t>
-  </si>
-  <si>
     <t>Funções da tela de carteira</t>
   </si>
   <si>
@@ -182,6 +173,21 @@
   </si>
   <si>
     <t>Funções da tela de despesas</t>
+  </si>
+  <si>
+    <t>Design da tela de receitas</t>
+  </si>
+  <si>
+    <t>Funções da tela de receitas</t>
+  </si>
+  <si>
+    <t>Funções da tela de perfil de usuário</t>
+  </si>
+  <si>
+    <t>Design da tela de estatísticas</t>
+  </si>
+  <si>
+    <t>Funções da tela de estatítsticas</t>
   </si>
 </sst>
 </file>
@@ -319,7 +325,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,7 +439,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -470,6 +475,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,13 +795,13 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.42578125" customWidth="1"/>
@@ -803,74 +809,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="A1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
       <c r="N2" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="31" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="24"/>
+      <c r="L3" s="23"/>
       <c r="N3" s="18" t="s">
         <v>37</v>
       </c>
       <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -895,10 +901,10 @@
       <c r="J4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="24"/>
+      <c r="L4" s="23"/>
       <c r="N4" s="19" t="s">
         <v>33</v>
       </c>
@@ -1112,7 +1118,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="15"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1131,7 +1137,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -1224,8 +1230,8 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
@@ -1262,13 +1268,13 @@
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
     <col min="3" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
@@ -1277,72 +1283,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="A1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
       <c r="N2" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="31" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="24"/>
+      <c r="L3" s="23"/>
       <c r="N3" s="18" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1367,10 +1373,10 @@
       <c r="J4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="24"/>
+      <c r="L4" s="23"/>
       <c r="N4" s="19" t="s">
         <v>33</v>
       </c>
@@ -1511,7 +1517,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1529,7 +1535,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="15"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1542,7 +1548,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1566,7 +1572,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1579,7 +1585,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1603,7 +1609,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1615,13 +1621,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1633,14 +1639,14 @@
         <v>15</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="14"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1651,14 +1657,14 @@
         <v>16</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="14"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="15"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1669,15 +1675,15 @@
         <v>17</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="14"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="5"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="7"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -1687,15 +1693,15 @@
         <v>18</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="14"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="5"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="7"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1705,7 +1711,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1713,8 +1719,8 @@
       <c r="F23" s="14"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="5"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="14"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
@@ -1722,15 +1728,17 @@
       <c r="A24" s="9">
         <v>20</v>
       </c>
-      <c r="B24" s="10"/>
+      <c r="B24" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="14"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="14"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
@@ -1738,7 +1746,9 @@
       <c r="A25" s="9">
         <v>21</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1746,8 +1756,8 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="14"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>